<commit_message>
Fixed nameing in 0195
</commit_message>
<xml_diff>
--- a/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Participant identifier schemes v4.xlsx
+++ b/peppol-id/src/test/resources/codelists/PEPPOL Code Lists - Participant identifier schemes v4.xlsx
@@ -895,9 +895,6 @@
     <t>0195</t>
   </si>
   <si>
-    <t>Singaport Nationwide E-Invoice Framework</t>
-  </si>
-  <si>
     <t>SG:UEN</t>
   </si>
   <si>
@@ -912,6 +909,9 @@
   </si>
   <si>
     <t>1) ICD 4 digits, 2) None</t>
+  </si>
+  <si>
+    <t>Singapore Nationwide E-Invoice Framework</t>
   </si>
 </sst>
 </file>
@@ -1424,8 +1424,8 @@
   <dimension ref="A1:J76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1796875" defaultRowHeight="14.5"/>
@@ -1693,13 +1693,13 @@
     </row>
     <row r="11" spans="1:10" ht="58">
       <c r="A11" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>269</v>
@@ -1709,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H11" s="8" t="s">
         <v>67</v>
@@ -1876,13 +1876,13 @@
     </row>
     <row r="19" spans="1:9" ht="29">
       <c r="A19" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>271</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>269</v>

</xml_diff>